<commit_message>
[IMP] Adjust GL Expenditure
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_gl_expenditure.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_gl_expenditure.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Expenditure" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Expenditure Report" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,27 +20,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
-  <si>
-    <t xml:space="preserve">Expenditure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activity Group Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activity Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">External Source of Fund Filters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost Center Filters</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+  <si>
+    <t xml:space="preserve">Expenditure Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investment Asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source of Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project (C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run By</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run Date</t>
   </si>
   <si>
     <t xml:space="preserve">Charge Type</t>
@@ -49,9 +88,6 @@
     <t xml:space="preserve">Fund Rule - Expense Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Account Code</t>
-  </si>
-  <si>
     <t xml:space="preserve">Account Name</t>
   </si>
   <si>
@@ -128,9 +164,6 @@
   </si>
   <si>
     <t xml:space="preserve">Source Doc/Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source of Fund</t>
   </si>
   <si>
     <t xml:space="preserve">Source of Budget Type</t>
@@ -315,7 +348,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,18 +377,38 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -365,18 +418,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BF13"/>
+  <dimension ref="A1:BF20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.95"/>
@@ -467,7 +520,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="X3" s="3"/>
@@ -482,10 +538,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="9"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="X4" s="3"/>
@@ -500,10 +556,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="X5" s="3"/>
@@ -518,10 +577,13 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="10"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="X6" s="3"/>
@@ -536,7 +598,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="3"/>
@@ -554,7 +616,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="3"/>
@@ -571,6 +633,10 @@
       <c r="BB8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -585,6 +651,10 @@
       <c r="BB9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="6"/>
       <c r="C10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -599,6 +669,10 @@
       <c r="BB10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="6"/>
       <c r="C11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -613,6 +687,10 @@
       <c r="BB11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -627,179 +705,301 @@
       <c r="BB12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AS13" s="3"/>
+      <c r="AV13" s="3"/>
+      <c r="AW13" s="3"/>
+      <c r="BB13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AS14" s="3"/>
+      <c r="AV14" s="3"/>
+      <c r="AW14" s="3"/>
+      <c r="BB14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AS15" s="3"/>
+      <c r="AV15" s="3"/>
+      <c r="AW15" s="3"/>
+      <c r="BB15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AS16" s="3"/>
+      <c r="AV16" s="3"/>
+      <c r="AW16" s="3"/>
+      <c r="BB16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AS17" s="3"/>
+      <c r="AV17" s="3"/>
+      <c r="AW17" s="3"/>
+      <c r="BB17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AS18" s="3"/>
+      <c r="AV18" s="3"/>
+      <c r="AW18" s="3"/>
+      <c r="BB18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AS19" s="3"/>
+      <c r="AV19" s="3"/>
+      <c r="AW19" s="3"/>
+      <c r="BB19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="7" t="s">
+      <c r="D20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="R20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="S20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="T20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="U20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="V20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="W20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="X20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y20" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC20" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="U13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="V13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="X13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC13" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="AN13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AP13" s="7" t="s">
+      <c r="AE20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AQ13" s="7" t="s">
+      <c r="AF20" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AR13" s="7" t="s">
+      <c r="AG20" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AS13" s="7" t="s">
+      <c r="AH20" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AT13" s="7" t="s">
+      <c r="AI20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="AU13" s="7" t="s">
+      <c r="AJ20" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AV13" s="7" t="s">
+      <c r="AK20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="AW13" s="7" t="s">
+      <c r="AL20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="AX13" s="7" t="s">
+      <c r="AM20" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="AY13" s="7" t="s">
+      <c r="AN20" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="AZ13" s="7" t="s">
+      <c r="AO20" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="BA13" s="7" t="s">
+      <c r="AP20" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="BB13" s="7" t="s">
+      <c r="AQ20" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="BC13" s="7" t="s">
+      <c r="AR20" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="BD13" s="7" t="s">
+      <c r="AS20" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="BE13" s="7" t="s">
+      <c r="AT20" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="BF13" s="7" t="s">
+      <c r="AU20" s="12" t="s">
         <v>64</v>
+      </c>
+      <c r="AV20" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AW20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AX20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="AY20" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AZ20" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="BA20" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB20" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="BC20" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="BD20" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE20" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="BF20" s="12" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>